<commit_message>
completando tabela de parâmetros
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/params.xlsx
+++ b/models/dissertation-model/modelo-R/params.xlsx
@@ -271,7 +271,7 @@
     <t xml:space="preserve">aDesiredMarketShare2</t>
   </si>
   <si>
-    <t xml:space="preserve">Market Share Desejado</t>
+    <t xml:space="preserve">Market Share Desejado* Na Estratégia Agressiva (talvez seja melhor separar)</t>
   </si>
   <si>
     <t xml:space="preserve">aSwitchForCapacityStrategy2</t>
@@ -460,12 +460,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -502,12 +508,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -534,23 +548,23 @@
   </sheetPr>
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.1224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="51.6836734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.9795918367347"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.0561224489796"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.6632653061225"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.6377551020408"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="11.9438775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="51.1632653061225"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.4744897959184"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="11.7448979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="8.77551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -610,9 +624,12 @@
       <c r="G2" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="H2" s="0"/>
       <c r="I2" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="J2" s="0"/>
+      <c r="K2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -636,9 +653,12 @@
       <c r="G3" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="H3" s="0"/>
       <c r="I3" s="1" t="n">
         <v>0.04</v>
       </c>
+      <c r="J3" s="0"/>
+      <c r="K3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -656,12 +676,16 @@
       <c r="E4" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="F4" s="0"/>
       <c r="G4" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="H4" s="0"/>
       <c r="I4" s="1" t="n">
         <v>0.25</v>
       </c>
+      <c r="J4" s="0"/>
+      <c r="K4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -691,12 +715,6 @@
       <c r="I5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="K5" s="1" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -705,14 +723,23 @@
       <c r="B6" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="C6" s="0"/>
+      <c r="D6" s="0"/>
       <c r="E6" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="F6" s="0"/>
       <c r="G6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I6" s="1" t="n">
         <v>0.1</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -722,15 +749,20 @@
       <c r="B7" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="C7" s="0"/>
+      <c r="D7" s="0"/>
       <c r="E7" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="F7" s="0"/>
       <c r="G7" s="1" t="s">
         <v>20</v>
       </c>
       <c r="I7" s="1" t="n">
         <v>0.001</v>
       </c>
+      <c r="J7" s="0"/>
+      <c r="K7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
@@ -739,15 +771,20 @@
       <c r="B8" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="C8" s="0"/>
+      <c r="D8" s="0"/>
       <c r="E8" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="F8" s="0"/>
       <c r="G8" s="1" t="s">
         <v>20</v>
       </c>
       <c r="I8" s="1" t="n">
         <v>1000</v>
       </c>
+      <c r="J8" s="0"/>
+      <c r="K8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
@@ -756,14 +793,23 @@
       <c r="B9" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="C9" s="0"/>
+      <c r="D9" s="0"/>
       <c r="E9" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="F9" s="0"/>
       <c r="G9" s="1" t="s">
         <v>39</v>
       </c>
       <c r="I9" s="1" t="n">
         <v>0.2</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -773,15 +819,20 @@
       <c r="B10" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="C10" s="0"/>
+      <c r="D10" s="0"/>
       <c r="E10" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="F10" s="0"/>
       <c r="G10" s="1" t="s">
         <v>20</v>
       </c>
       <c r="I10" s="1" t="n">
         <v>60000000</v>
       </c>
+      <c r="J10" s="0"/>
+      <c r="K10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
@@ -790,15 +841,20 @@
       <c r="B11" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="C11" s="0"/>
+      <c r="D11" s="0"/>
       <c r="E11" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="F11" s="0"/>
       <c r="G11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I11" s="1" t="n">
         <v>0.001</v>
       </c>
+      <c r="J11" s="0"/>
+      <c r="K11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
@@ -807,15 +863,20 @@
       <c r="B12" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="C12" s="0"/>
+      <c r="D12" s="0"/>
       <c r="E12" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="F12" s="0"/>
       <c r="G12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I12" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="J12" s="0"/>
+      <c r="K12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
@@ -824,15 +885,20 @@
       <c r="B13" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="C13" s="0"/>
+      <c r="D13" s="0"/>
       <c r="E13" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="F13" s="0"/>
       <c r="G13" s="1" t="s">
         <v>20</v>
       </c>
       <c r="I13" s="1" t="n">
         <v>100000000</v>
       </c>
+      <c r="J13" s="0"/>
+      <c r="K13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
@@ -847,6 +913,7 @@
       <c r="D14" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E14" s="0"/>
       <c r="F14" s="1" t="s">
         <v>27</v>
       </c>
@@ -854,12 +921,6 @@
         <v>20</v>
       </c>
       <c r="I14" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K14" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -885,6 +946,12 @@
       <c r="I15" s="1" t="n">
         <v>0.25</v>
       </c>
+      <c r="J15" s="1" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="K15" s="1" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
@@ -931,6 +998,12 @@
       <c r="I17" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="J17" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K17" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
@@ -939,6 +1012,8 @@
       <c r="B18" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="C18" s="0"/>
+      <c r="D18" s="0"/>
       <c r="E18" s="1" t="s">
         <v>23</v>
       </c>
@@ -956,6 +1031,8 @@
       <c r="B19" s="1" t="s">
         <v>60</v>
       </c>
+      <c r="C19" s="0"/>
+      <c r="D19" s="0"/>
       <c r="E19" s="1" t="s">
         <v>23</v>
       </c>
@@ -973,6 +1050,8 @@
       <c r="B20" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="C20" s="0"/>
+      <c r="D20" s="0"/>
       <c r="E20" s="1" t="s">
         <v>18</v>
       </c>
@@ -990,6 +1069,8 @@
       <c r="B21" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="C21" s="0"/>
+      <c r="D21" s="0"/>
       <c r="E21" s="1" t="s">
         <v>18</v>
       </c>
@@ -998,6 +1079,12 @@
       </c>
       <c r="I21" s="1" t="n">
         <v>-8</v>
+      </c>
+      <c r="J21" s="1" t="n">
+        <v>-12</v>
+      </c>
+      <c r="K21" s="1" t="n">
+        <v>-4</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1007,6 +1094,8 @@
       <c r="B22" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="C22" s="0"/>
+      <c r="D22" s="0"/>
       <c r="E22" s="1" t="s">
         <v>33</v>
       </c>
@@ -1021,6 +1110,8 @@
       <c r="B23" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="C23" s="0"/>
+      <c r="D23" s="0"/>
       <c r="E23" s="1" t="s">
         <v>69</v>
       </c>
@@ -1035,10 +1126,19 @@
       <c r="B24" s="1" t="s">
         <v>71</v>
       </c>
+      <c r="C24" s="0"/>
+      <c r="D24" s="0"/>
       <c r="E24" s="1" t="s">
         <v>18</v>
       </c>
       <c r="I24" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J24" s="1" t="n">
+        <f aca="false">1/3</f>
+        <v>0.333333333333333</v>
+      </c>
+      <c r="K24" s="1" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1049,6 +1149,8 @@
       <c r="B25" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="C25" s="0"/>
+      <c r="D25" s="0"/>
       <c r="E25" s="1" t="s">
         <v>36</v>
       </c>
@@ -1063,6 +1165,8 @@
       <c r="B26" s="1" t="s">
         <v>75</v>
       </c>
+      <c r="C26" s="0"/>
+      <c r="D26" s="0"/>
       <c r="E26" s="1" t="s">
         <v>33</v>
       </c>
@@ -1077,20 +1181,30 @@
       <c r="B27" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="C27" s="0"/>
+      <c r="D27" s="0"/>
       <c r="E27" s="1" t="s">
         <v>33</v>
       </c>
       <c r="I27" s="1" t="n">
         <v>0.8</v>
       </c>
+      <c r="J27" s="1" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="K27" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>79</v>
       </c>
+      <c r="C28" s="0"/>
+      <c r="D28" s="0"/>
       <c r="E28" s="1" t="s">
         <v>80</v>
       </c>
@@ -1105,11 +1219,19 @@
       <c r="B29" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="C29" s="0"/>
+      <c r="D29" s="0"/>
       <c r="E29" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I29" s="1" t="n">
+      <c r="I29" s="3" t="n">
         <v>0.5</v>
+      </c>
+      <c r="J29" s="3" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="K29" s="3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1125,6 +1247,7 @@
       <c r="D30" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="E30" s="0"/>
       <c r="I30" s="1" t="n">
         <v>1</v>
       </c>
@@ -1136,6 +1259,7 @@
       <c r="B31" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="E31" s="0"/>
       <c r="I31" s="1" t="n">
         <v>1</v>
       </c>
@@ -1181,6 +1305,12 @@
       <c r="I34" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="J34" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K34" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
@@ -1195,6 +1325,12 @@
       <c r="I35" s="1" t="n">
         <v>0.25</v>
       </c>
+      <c r="J35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K35" s="1" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
@@ -1208,6 +1344,12 @@
       </c>
       <c r="I36" s="1" t="n">
         <v>-0.1</v>
+      </c>
+      <c r="J36" s="1" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="K36" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1245,11 +1387,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.66836734693878"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.3061224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.53571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="8.77551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1338,11 +1480,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="0" t="s">
@@ -1387,11 +1529,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.7448979591837"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.780612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.4744897959184"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.3724489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
modelo rodando com dados do excel
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/params.xlsx
+++ b/models/dissertation-model/modelo-R/params.xlsx
@@ -428,7 +428,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -450,6 +450,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -508,12 +516,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -525,7 +537,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -548,57 +560,57 @@
   </sheetPr>
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="30.780612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="51.1632653061225"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.4744897959184"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="11.7448979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.7040816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="50.484693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.1734693877551"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="11.4744897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -610,10 +622,12 @@
         <v>12</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>0.5</v>
+        <f aca="false">MAX(I2,J2)</f>
+        <v>1</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>3</v>
+        <f aca="false">MAX(I2,K2)</f>
+        <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>13</v>
@@ -639,9 +653,11 @@
         <v>17</v>
       </c>
       <c r="C3" s="1" t="n">
+        <f aca="false">MAX(I3,J3)</f>
         <v>0.04</v>
       </c>
       <c r="D3" s="1" t="n">
+        <f aca="false">MAX(I3,K3)</f>
         <v>0.04</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -668,9 +684,11 @@
         <v>22</v>
       </c>
       <c r="C4" s="1" t="n">
+        <f aca="false">MAX(I4,J4)</f>
         <v>0.25</v>
       </c>
       <c r="D4" s="1" t="n">
+        <f aca="false">MAX(I4,K4)</f>
         <v>0.25</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -695,9 +713,11 @@
         <v>25</v>
       </c>
       <c r="C5" s="1" t="n">
+        <f aca="false">MAX(I5,J5)</f>
         <v>1</v>
       </c>
       <c r="D5" s="1" t="n">
+        <f aca="false">MAX(I5,K5)</f>
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -715,6 +735,8 @@
       <c r="I5" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="J5" s="0"/>
+      <c r="K5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -723,8 +745,14 @@
       <c r="B6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="0"/>
-      <c r="D6" s="0"/>
+      <c r="C6" s="1" t="n">
+        <f aca="false">MAX(I6,J6)</f>
+        <v>0.1</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <f aca="false">MAX(I6,K6)</f>
+        <v>0.5</v>
+      </c>
       <c r="E6" s="1" t="s">
         <v>30</v>
       </c>
@@ -749,8 +777,14 @@
       <c r="B7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="0"/>
-      <c r="D7" s="0"/>
+      <c r="C7" s="1" t="n">
+        <f aca="false">MAX(I7,J7)</f>
+        <v>0.001</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <f aca="false">MAX(I7,K7)</f>
+        <v>0.001</v>
+      </c>
       <c r="E7" s="1" t="s">
         <v>33</v>
       </c>
@@ -771,8 +805,14 @@
       <c r="B8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="0"/>
-      <c r="D8" s="0"/>
+      <c r="C8" s="1" t="n">
+        <f aca="false">MAX(I8,J8)</f>
+        <v>1000</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <f aca="false">MAX(I8,K8)</f>
+        <v>1000</v>
+      </c>
       <c r="E8" s="1" t="s">
         <v>36</v>
       </c>
@@ -793,8 +833,14 @@
       <c r="B9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="0"/>
-      <c r="D9" s="0"/>
+      <c r="C9" s="1" t="n">
+        <f aca="false">MAX(I9,J9)</f>
+        <v>0.2</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <f aca="false">MAX(I9,K9)</f>
+        <v>1</v>
+      </c>
       <c r="E9" s="1" t="s">
         <v>39</v>
       </c>
@@ -819,8 +865,14 @@
       <c r="B10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="0"/>
-      <c r="D10" s="0"/>
+      <c r="C10" s="1" t="n">
+        <f aca="false">MAX(I10,J10)</f>
+        <v>60000000</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <f aca="false">MAX(I10,K10)</f>
+        <v>60000000</v>
+      </c>
       <c r="E10" s="1" t="s">
         <v>42</v>
       </c>
@@ -841,8 +893,14 @@
       <c r="B11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="0"/>
-      <c r="D11" s="0"/>
+      <c r="C11" s="1" t="n">
+        <f aca="false">MAX(I11,J11)</f>
+        <v>0.001</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <f aca="false">MAX(I11,K11)</f>
+        <v>0.001</v>
+      </c>
       <c r="E11" s="1" t="s">
         <v>33</v>
       </c>
@@ -863,8 +921,14 @@
       <c r="B12" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="0"/>
-      <c r="D12" s="0"/>
+      <c r="C12" s="1" t="n">
+        <f aca="false">MAX(I12,J12)</f>
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <f aca="false">MAX(I12,K12)</f>
+        <v>1</v>
+      </c>
       <c r="E12" s="1" t="s">
         <v>39</v>
       </c>
@@ -885,8 +949,14 @@
       <c r="B13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="0"/>
-      <c r="D13" s="0"/>
+      <c r="C13" s="1" t="n">
+        <f aca="false">MAX(I13,J13)</f>
+        <v>100000000</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <f aca="false">MAX(I13,K13)</f>
+        <v>100000000</v>
+      </c>
       <c r="E13" s="1" t="s">
         <v>42</v>
       </c>
@@ -908,9 +978,11 @@
         <v>50</v>
       </c>
       <c r="C14" s="1" t="n">
+        <f aca="false">MAX(I14,J14)</f>
         <v>0</v>
       </c>
       <c r="D14" s="1" t="n">
+        <f aca="false">MAX(I14,K14)</f>
         <v>0</v>
       </c>
       <c r="E14" s="0"/>
@@ -923,6 +995,8 @@
       <c r="I14" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="J14" s="0"/>
+      <c r="K14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
@@ -932,9 +1006,11 @@
         <v>52</v>
       </c>
       <c r="C15" s="1" t="n">
+        <f aca="false">MAX(I15,J15)</f>
         <v>0.25</v>
       </c>
       <c r="D15" s="1" t="n">
+        <f aca="false">MAX(I15,K15)</f>
         <v>0.25</v>
       </c>
       <c r="E15" s="1" t="s">
@@ -961,9 +1037,11 @@
         <v>54</v>
       </c>
       <c r="C16" s="1" t="n">
+        <f aca="false">MAX(I16,J16)</f>
         <v>1</v>
       </c>
       <c r="D16" s="1" t="n">
+        <f aca="false">MAX(I16,K16)</f>
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
@@ -975,6 +1053,8 @@
       <c r="I16" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="J16" s="0"/>
+      <c r="K16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
@@ -984,9 +1064,11 @@
         <v>56</v>
       </c>
       <c r="C17" s="1" t="n">
+        <f aca="false">MAX(I17,J17)</f>
         <v>1</v>
       </c>
       <c r="D17" s="1" t="n">
+        <f aca="false">MAX(I17,K17)</f>
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
@@ -1012,8 +1094,14 @@
       <c r="B18" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="0"/>
-      <c r="D18" s="0"/>
+      <c r="C18" s="1" t="n">
+        <f aca="false">MAX(I18,J18)</f>
+        <v>1</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <f aca="false">MAX(I18,K18)</f>
+        <v>1</v>
+      </c>
       <c r="E18" s="1" t="s">
         <v>23</v>
       </c>
@@ -1023,6 +1111,8 @@
       <c r="I18" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="J18" s="0"/>
+      <c r="K18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
@@ -1031,8 +1121,14 @@
       <c r="B19" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="0"/>
-      <c r="D19" s="0"/>
+      <c r="C19" s="1" t="n">
+        <f aca="false">MAX(I19,J19)</f>
+        <v>0.25</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <f aca="false">MAX(I19,K19)</f>
+        <v>0.25</v>
+      </c>
       <c r="E19" s="1" t="s">
         <v>23</v>
       </c>
@@ -1042,6 +1138,8 @@
       <c r="I19" s="1" t="n">
         <v>0.25</v>
       </c>
+      <c r="J19" s="0"/>
+      <c r="K19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
@@ -1050,8 +1148,14 @@
       <c r="B20" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="0"/>
-      <c r="D20" s="0"/>
+      <c r="C20" s="1" t="n">
+        <f aca="false">MAX(I20,J20)</f>
+        <v>-4</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <f aca="false">MAX(I20,K20)</f>
+        <v>-4</v>
+      </c>
       <c r="E20" s="1" t="s">
         <v>18</v>
       </c>
@@ -1061,6 +1165,8 @@
       <c r="I20" s="1" t="n">
         <v>-4</v>
       </c>
+      <c r="J20" s="0"/>
+      <c r="K20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
@@ -1069,8 +1175,14 @@
       <c r="B21" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C21" s="0"/>
-      <c r="D21" s="0"/>
+      <c r="C21" s="1" t="n">
+        <f aca="false">MAX(I21,J21)</f>
+        <v>-8</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <f aca="false">MAX(I21,K21)</f>
+        <v>-4</v>
+      </c>
       <c r="E21" s="1" t="s">
         <v>18</v>
       </c>
@@ -1094,14 +1206,22 @@
       <c r="B22" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C22" s="0"/>
-      <c r="D22" s="0"/>
+      <c r="C22" s="1" t="n">
+        <f aca="false">MAX(I22,J22)</f>
+        <v>0.7</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <f aca="false">MAX(I22,K22)</f>
+        <v>0.7</v>
+      </c>
       <c r="E22" s="1" t="s">
         <v>33</v>
       </c>
       <c r="I22" s="1" t="n">
         <v>0.7</v>
       </c>
+      <c r="J22" s="0"/>
+      <c r="K22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
@@ -1110,14 +1230,22 @@
       <c r="B23" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C23" s="0"/>
-      <c r="D23" s="0"/>
+      <c r="C23" s="1" t="n">
+        <f aca="false">MAX(I23,J23)</f>
+        <v>10000000</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <f aca="false">MAX(I23,K23)</f>
+        <v>10000000</v>
+      </c>
       <c r="E23" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I23" s="1" t="n">
         <v>10000000</v>
       </c>
+      <c r="J23" s="0"/>
+      <c r="K23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
@@ -1126,8 +1254,14 @@
       <c r="B24" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C24" s="0"/>
-      <c r="D24" s="0"/>
+      <c r="C24" s="1" t="n">
+        <f aca="false">MAX(I24,J24)</f>
+        <v>3</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <f aca="false">MAX(I24,K24)</f>
+        <v>3</v>
+      </c>
       <c r="E24" s="1" t="s">
         <v>18</v>
       </c>
@@ -1149,14 +1283,22 @@
       <c r="B25" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C25" s="0"/>
-      <c r="D25" s="0"/>
+      <c r="C25" s="1" t="n">
+        <f aca="false">MAX(I25,J25)</f>
+        <v>1000</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <f aca="false">MAX(I25,K25)</f>
+        <v>1000</v>
+      </c>
       <c r="E25" s="1" t="s">
         <v>36</v>
       </c>
       <c r="I25" s="1" t="n">
         <v>1000</v>
       </c>
+      <c r="J25" s="0"/>
+      <c r="K25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
@@ -1165,14 +1307,22 @@
       <c r="B26" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C26" s="0"/>
-      <c r="D26" s="0"/>
+      <c r="C26" s="1" t="n">
+        <f aca="false">MAX(I26,J26)</f>
+        <v>0.2</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <f aca="false">MAX(I26,K26)</f>
+        <v>0.2</v>
+      </c>
       <c r="E26" s="1" t="s">
         <v>33</v>
       </c>
       <c r="I26" s="1" t="n">
         <v>0.2</v>
       </c>
+      <c r="J26" s="0"/>
+      <c r="K26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
@@ -1181,8 +1331,14 @@
       <c r="B27" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C27" s="0"/>
-      <c r="D27" s="0"/>
+      <c r="C27" s="1" t="n">
+        <f aca="false">MAX(I27,J27)</f>
+        <v>0.8</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <f aca="false">MAX(I27,K27)</f>
+        <v>1</v>
+      </c>
       <c r="E27" s="1" t="s">
         <v>33</v>
       </c>
@@ -1197,20 +1353,28 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="3" t="s">
         <v>78</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C28" s="0"/>
-      <c r="D28" s="0"/>
+      <c r="C28" s="1" t="n">
+        <f aca="false">MAX(I28,J28)</f>
+        <v>100000</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <f aca="false">MAX(I28,K28)</f>
+        <v>100000</v>
+      </c>
       <c r="E28" s="1" t="s">
         <v>80</v>
       </c>
       <c r="I28" s="1" t="n">
         <v>100000</v>
       </c>
+      <c r="J28" s="0"/>
+      <c r="K28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
@@ -1219,18 +1383,24 @@
       <c r="B29" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C29" s="0"/>
-      <c r="D29" s="0"/>
+      <c r="C29" s="1" t="n">
+        <f aca="false">MAX(I29,J29)</f>
+        <v>0.6</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <f aca="false">MAX(I29,K29)</f>
+        <v>1</v>
+      </c>
       <c r="E29" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I29" s="3" t="n">
+      <c r="I29" s="4" t="n">
         <v>0.5</v>
       </c>
-      <c r="J29" s="3" t="n">
+      <c r="J29" s="4" t="n">
         <v>0.6</v>
       </c>
-      <c r="K29" s="3" t="n">
+      <c r="K29" s="4" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1242,15 +1412,19 @@
         <v>84</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>0</v>
+        <f aca="false">MAX(I30,J30)</f>
+        <v>1</v>
       </c>
       <c r="D30" s="1" t="n">
+        <f aca="false">MAX(I30,K30)</f>
         <v>1</v>
       </c>
       <c r="E30" s="0"/>
       <c r="I30" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="J30" s="0"/>
+      <c r="K30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
@@ -1259,10 +1433,20 @@
       <c r="B31" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="C31" s="1" t="n">
+        <f aca="false">MAX(I31,J31)</f>
+        <v>1</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <f aca="false">MAX(I31,K31)</f>
+        <v>1</v>
+      </c>
       <c r="E31" s="0"/>
       <c r="I31" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="J31" s="0"/>
+      <c r="K31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
@@ -1271,12 +1455,22 @@
       <c r="B32" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="C32" s="1" t="n">
+        <f aca="false">MAX(I32,J32)</f>
+        <v>0.25</v>
+      </c>
+      <c r="D32" s="1" t="n">
+        <f aca="false">MAX(I32,K32)</f>
+        <v>0.25</v>
+      </c>
       <c r="E32" s="1" t="s">
         <v>23</v>
       </c>
       <c r="I32" s="1" t="n">
         <v>0.25</v>
       </c>
+      <c r="J32" s="0"/>
+      <c r="K32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
@@ -1285,12 +1479,22 @@
       <c r="B33" s="1" t="s">
         <v>89</v>
       </c>
+      <c r="C33" s="1" t="n">
+        <f aca="false">MAX(I33,J33)</f>
+        <v>0.25</v>
+      </c>
+      <c r="D33" s="1" t="n">
+        <f aca="false">MAX(I33,K33)</f>
+        <v>0.25</v>
+      </c>
       <c r="E33" s="1" t="s">
         <v>23</v>
       </c>
       <c r="I33" s="1" t="n">
         <v>0.25</v>
       </c>
+      <c r="J33" s="0"/>
+      <c r="K33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
@@ -1299,6 +1503,14 @@
       <c r="B34" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="C34" s="1" t="n">
+        <f aca="false">MAX(I34,J34)</f>
+        <v>1</v>
+      </c>
+      <c r="D34" s="1" t="n">
+        <f aca="false">MAX(I34,K34)</f>
+        <v>1</v>
+      </c>
       <c r="E34" s="1" t="s">
         <v>18</v>
       </c>
@@ -1319,6 +1531,14 @@
       <c r="B35" s="1" t="s">
         <v>93</v>
       </c>
+      <c r="C35" s="1" t="n">
+        <f aca="false">MAX(I35,J35)</f>
+        <v>0.25</v>
+      </c>
+      <c r="D35" s="1" t="n">
+        <f aca="false">MAX(I35,K35)</f>
+        <v>0.25</v>
+      </c>
       <c r="E35" s="1" t="s">
         <v>18</v>
       </c>
@@ -1339,6 +1559,14 @@
       <c r="B36" s="1" t="s">
         <v>95</v>
       </c>
+      <c r="C36" s="1" t="n">
+        <f aca="false">MAX(I36,J36)</f>
+        <v>-0.1</v>
+      </c>
+      <c r="D36" s="1" t="n">
+        <f aca="false">MAX(I36,K36)</f>
+        <v>0</v>
+      </c>
       <c r="E36" s="1" t="s">
         <v>18</v>
       </c>
@@ -1358,6 +1586,14 @@
       </c>
       <c r="B37" s="1" t="s">
         <v>97</v>
+      </c>
+      <c r="C37" s="1" t="n">
+        <f aca="false">MAX(I37,J37)</f>
+        <v>0</v>
+      </c>
+      <c r="D37" s="1" t="n">
+        <f aca="false">MAX(I37,K37)</f>
+        <v>0</v>
       </c>
       <c r="I37" s="1" t="n">
         <v>0</v>
@@ -1381,17 +1617,17 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.53571428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.39795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1474,17 +1710,17 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="0" t="s">
@@ -1523,17 +1759,17 @@
   </sheetPr>
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.4744897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.3724489795918"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
análise RDM rodando no modelo do Sterman!!
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/params.xlsx
+++ b/models/dissertation-model/modelo-R/params.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" state="visible" r:id="rId2"/>
@@ -560,23 +560,23 @@
   </sheetPr>
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.7040816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="50.484693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.1734693877551"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="11.4744897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="30.9132653061224"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="49.2704081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1416,8 +1416,7 @@
         <v>1</v>
       </c>
       <c r="D30" s="1" t="n">
-        <f aca="false">MAX(I30,K30)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E30" s="0"/>
       <c r="I30" s="1" t="n">
@@ -1615,19 +1614,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.39795918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.12755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="25.3877551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1644,54 +1643,173 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="str">
-        <f aca="false">"ADV-"&amp;D2</f>
-        <v>ADV-0,5</v>
+        <f aca="false">"C."&amp;C2&amp;"-."&amp;D2</f>
+        <v>C.1-.0,5</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
+        <f aca="false">A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="1" t="str">
-        <f aca="false">"ADV-"&amp;D3</f>
-        <v>ADV-0,5</v>
+        <f aca="false">"C."&amp;C3&amp;"-."&amp;D3</f>
+        <v>C.1-.0,6</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="n">
+        <f aca="false">D2+0.1</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <f aca="false">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="str">
+        <f aca="false">"C."&amp;C4&amp;"-."&amp;D4</f>
+        <v>C.1-.0,7</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <f aca="false">D3+0.1</f>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <f aca="false">A4+1</f>
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="str">
+        <f aca="false">"C."&amp;C5&amp;"-."&amp;D5</f>
+        <v>C.1-.0,8</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <f aca="false">D4+0.1</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <f aca="false">A5+1</f>
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="str">
+        <f aca="false">"C."&amp;C6&amp;"-."&amp;D6</f>
+        <v>C.1-.0,9</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <f aca="false">D5+0.1</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <f aca="false">A6+1</f>
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="str">
+        <f aca="false">"C."&amp;C7&amp;"-."&amp;D7</f>
+        <v>C.2-.0,5</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <f aca="false">D2</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <f aca="false">A7+1</f>
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="str">
+        <f aca="false">"C."&amp;C8&amp;"-."&amp;D8</f>
+        <v>C.2-.0,6</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <f aca="false">D3</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <f aca="false">A8+1</f>
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="str">
+        <f aca="false">"C."&amp;C9&amp;"-."&amp;D9</f>
+        <v>C.2-.0,7</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <f aca="false">D4</f>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <f aca="false">A9+1</f>
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="str">
+        <f aca="false">"C."&amp;C10&amp;"-."&amp;D10</f>
+        <v>C.2-.0,8</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <f aca="false">D5</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="str">
+        <f aca="false">"C."&amp;C11&amp;"-."&amp;D11</f>
+        <v>C.2-.0,9</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <f aca="false">D6</f>
+        <v>0.9</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1710,14 +1828,11 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
@@ -1759,17 +1874,16 @@
   </sheetPr>
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.1020408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.2908163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.0918367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
corrigindo problema nas variáveis globais
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/params.xlsx
+++ b/models/dissertation-model/modelo-R/params.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="133">
   <si>
     <t xml:space="preserve">Variavel</t>
   </si>
@@ -58,6 +58,9 @@
     <t xml:space="preserve">Sterman Max</t>
   </si>
   <si>
+    <t xml:space="preserve">Igual</t>
+  </si>
+  <si>
     <t xml:space="preserve">aUnitsPerHousehold</t>
   </si>
   <si>
@@ -76,7 +79,7 @@
     <t xml:space="preserve">aDiscountRate</t>
   </si>
   <si>
-    <t xml:space="preserve">Taxa de Disconto</t>
+    <t xml:space="preserve">Taxa de Desconto</t>
   </si>
   <si>
     <t xml:space="preserve">adimensional</t>
@@ -516,7 +519,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -526,6 +529,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -558,25 +565,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="48.1938775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="46.9795918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="7.69387755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -613,30 +620,32 @@
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="n">
         <f aca="false">MAX(I2,J2)</f>
         <v>1</v>
       </c>
       <c r="D2" s="1" t="n">
-        <f aca="false">MAX(I2,K2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H2" s="0"/>
       <c r="I2" s="1" t="n">
@@ -644,13 +653,17 @@
       </c>
       <c r="J2" s="0"/>
       <c r="K2" s="0"/>
+      <c r="L2" s="3" t="n">
+        <f aca="false">C2=D2</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="n">
         <f aca="false">MAX(I3,J3)</f>
@@ -661,13 +674,13 @@
         <v>0.04</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H3" s="0"/>
       <c r="I3" s="1" t="n">
@@ -675,13 +688,17 @@
       </c>
       <c r="J3" s="0"/>
       <c r="K3" s="0"/>
+      <c r="L3" s="3" t="n">
+        <f aca="false">C3=D3</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C4" s="1" t="n">
         <f aca="false">MAX(I4,J4)</f>
@@ -692,11 +709,11 @@
         <v>0.25</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F4" s="0"/>
       <c r="G4" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H4" s="0"/>
       <c r="I4" s="1" t="n">
@@ -704,13 +721,17 @@
       </c>
       <c r="J4" s="0"/>
       <c r="K4" s="0"/>
+      <c r="L4" s="3" t="n">
+        <f aca="false">C4=D4</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C5" s="1" t="n">
         <f aca="false">MAX(I5,J5)</f>
@@ -721,13 +742,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H5" s="1" t="n">
         <v>1</v>
@@ -737,13 +758,17 @@
       </c>
       <c r="J5" s="0"/>
       <c r="K5" s="0"/>
+      <c r="L5" s="3" t="n">
+        <f aca="false">C5=D5</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C6" s="1" t="n">
         <f aca="false">MAX(I6,J6)</f>
@@ -754,11 +779,11 @@
         <v>0.5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F6" s="0"/>
       <c r="G6" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I6" s="1" t="n">
         <v>0.1</v>
@@ -769,13 +794,17 @@
       <c r="K6" s="0" t="n">
         <v>0.5</v>
       </c>
+      <c r="L6" s="3" t="n">
+        <f aca="false">C6=D6</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C7" s="1" t="n">
         <f aca="false">MAX(I7,J7)</f>
@@ -786,52 +815,58 @@
         <v>0.001</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F7" s="0"/>
       <c r="G7" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I7" s="1" t="n">
         <v>0.001</v>
       </c>
       <c r="J7" s="0"/>
       <c r="K7" s="0"/>
+      <c r="L7" s="3" t="n">
+        <f aca="false">C7=D7</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C8" s="1" t="n">
-        <f aca="false">MAX(I8,J8)</f>
-        <v>1000</v>
+        <v>7000</v>
       </c>
       <c r="D8" s="1" t="n">
-        <f aca="false">MAX(I8,K8)</f>
-        <v>1000</v>
+        <v>7000</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F8" s="0"/>
       <c r="G8" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I8" s="1" t="n">
         <v>1000</v>
       </c>
       <c r="J8" s="0"/>
       <c r="K8" s="0"/>
+      <c r="L8" s="3" t="n">
+        <f aca="false">C8=D8</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C9" s="1" t="n">
         <f aca="false">MAX(I9,J9)</f>
@@ -842,11 +877,11 @@
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F9" s="0"/>
       <c r="G9" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I9" s="1" t="n">
         <v>0.2</v>
@@ -857,41 +892,47 @@
       <c r="K9" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="L9" s="3" t="n">
+        <f aca="false">C9=D9</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C10" s="1" t="n">
-        <f aca="false">MAX(I10,J10)</f>
-        <v>60000000</v>
+        <v>200000</v>
       </c>
       <c r="D10" s="1" t="n">
-        <f aca="false">MAX(I10,K10)</f>
-        <v>60000000</v>
+        <v>200000</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F10" s="0"/>
       <c r="G10" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I10" s="1" t="n">
         <v>60000000</v>
       </c>
       <c r="J10" s="0"/>
       <c r="K10" s="0"/>
+      <c r="L10" s="3" t="n">
+        <f aca="false">C10=D10</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C11" s="1" t="n">
         <f aca="false">MAX(I11,J11)</f>
@@ -902,24 +943,28 @@
         <v>0.001</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F11" s="0"/>
       <c r="G11" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I11" s="1" t="n">
         <v>0.001</v>
       </c>
       <c r="J11" s="0"/>
       <c r="K11" s="0"/>
+      <c r="L11" s="3" t="n">
+        <f aca="false">C11=D11</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C12" s="1" t="n">
         <f aca="false">MAX(I12,J12)</f>
@@ -930,52 +975,60 @@
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F12" s="0"/>
       <c r="G12" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I12" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J12" s="0"/>
       <c r="K12" s="0"/>
+      <c r="L12" s="3" t="n">
+        <f aca="false">C12=D12</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C13" s="1" t="n">
-        <f aca="false">MAX(I13,J13)</f>
-        <v>100000000</v>
+        <f aca="false">C10*5</f>
+        <v>1000000</v>
       </c>
       <c r="D13" s="1" t="n">
-        <f aca="false">MAX(I13,K13)</f>
-        <v>100000000</v>
+        <f aca="false">D10*5</f>
+        <v>1000000</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F13" s="0"/>
       <c r="G13" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I13" s="1" t="n">
         <v>100000000</v>
       </c>
       <c r="J13" s="0"/>
       <c r="K13" s="0"/>
+      <c r="L13" s="3" t="n">
+        <f aca="false">C13=D13</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C14" s="1" t="n">
         <f aca="false">MAX(I14,J14)</f>
@@ -987,37 +1040,39 @@
       </c>
       <c r="E14" s="0"/>
       <c r="F14" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I14" s="1" t="n">
         <v>0</v>
       </c>
       <c r="J14" s="0"/>
       <c r="K14" s="0"/>
+      <c r="L14" s="3" t="n">
+        <f aca="false">C14=D14</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C15" s="1" t="n">
-        <f aca="false">MAX(I15,J15)</f>
+        <v>0.125</v>
+      </c>
+      <c r="D15" s="1" t="n">
         <v>0.25</v>
       </c>
-      <c r="D15" s="1" t="n">
-        <f aca="false">MAX(I15,K15)</f>
-        <v>0.25</v>
-      </c>
       <c r="E15" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I15" s="1" t="n">
         <v>0.25</v>
@@ -1028,13 +1083,17 @@
       <c r="K15" s="1" t="n">
         <v>0.25</v>
       </c>
+      <c r="L15" s="3" t="n">
+        <f aca="false">C15=D15</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C16" s="1" t="n">
         <f aca="false">MAX(I16,J16)</f>
@@ -1045,37 +1104,39 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I16" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J16" s="0"/>
       <c r="K16" s="0"/>
+      <c r="L16" s="3" t="n">
+        <f aca="false">C16=D16</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C17" s="1" t="n">
-        <f aca="false">MAX(I17,J17)</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D17" s="1" t="n">
-        <f aca="false">MAX(I17,K17)</f>
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I17" s="1" t="n">
         <v>1</v>
@@ -1086,13 +1147,17 @@
       <c r="K17" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="L17" s="3" t="n">
+        <f aca="false">C17=D17</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C18" s="1" t="n">
         <f aca="false">MAX(I18,J18)</f>
@@ -1103,23 +1168,27 @@
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I18" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J18" s="0"/>
       <c r="K18" s="0"/>
+      <c r="L18" s="3" t="n">
+        <f aca="false">C18=D18</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C19" s="1" t="n">
         <f aca="false">MAX(I19,J19)</f>
@@ -1130,64 +1199,69 @@
         <v>0.25</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I19" s="1" t="n">
         <v>0.25</v>
       </c>
       <c r="J19" s="0"/>
       <c r="K19" s="0"/>
+      <c r="L19" s="3" t="n">
+        <f aca="false">C19=D19</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C20" s="1" t="n">
-        <f aca="false">MAX(I20,J20)</f>
-        <v>-4</v>
+        <v>-12</v>
       </c>
       <c r="D20" s="1" t="n">
         <f aca="false">MAX(I20,K20)</f>
         <v>-4</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I20" s="1" t="n">
         <v>-4</v>
       </c>
       <c r="J20" s="0"/>
       <c r="K20" s="0"/>
+      <c r="L20" s="3" t="n">
+        <f aca="false">C20=D20</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C21" s="1" t="n">
-        <f aca="false">MAX(I21,J21)</f>
-        <v>-8</v>
+        <v>-12</v>
       </c>
       <c r="D21" s="1" t="n">
-        <f aca="false">MAX(I21,K21)</f>
         <v>-4</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I21" s="1" t="n">
         <v>-8</v>
@@ -1198,72 +1272,81 @@
       <c r="K21" s="1" t="n">
         <v>-4</v>
       </c>
+      <c r="L21" s="3" t="n">
+        <f aca="false">C21=D21</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C22" s="1" t="n">
-        <f aca="false">MAX(I22,J22)</f>
         <v>0.7</v>
       </c>
       <c r="D22" s="1" t="n">
-        <f aca="false">MAX(I22,K22)</f>
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I22" s="1" t="n">
         <v>0.7</v>
       </c>
       <c r="J22" s="0"/>
       <c r="K22" s="0"/>
+      <c r="L22" s="3" t="n">
+        <f aca="false">C22=D22</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C23" s="1" t="n">
-        <f aca="false">MAX(I23,J23)</f>
-        <v>10000000</v>
+        <f aca="false">C13</f>
+        <v>1000000</v>
       </c>
       <c r="D23" s="1" t="n">
-        <f aca="false">MAX(I23,K23)</f>
-        <v>10000000</v>
+        <f aca="false">D13</f>
+        <v>1000000</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I23" s="1" t="n">
         <v>10000000</v>
       </c>
       <c r="J23" s="0"/>
       <c r="K23" s="0"/>
+      <c r="L23" s="3" t="n">
+        <f aca="false">C23=D23</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C24" s="1" t="n">
-        <f aca="false">MAX(I24,J24)</f>
-        <v>3</v>
+        <v>0.333</v>
       </c>
       <c r="D24" s="1" t="n">
         <f aca="false">MAX(I24,K24)</f>
         <v>3</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I24" s="1" t="n">
         <v>3</v>
@@ -1275,37 +1358,43 @@
       <c r="K24" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="L24" s="3" t="n">
+        <f aca="false">C24=D24</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C25" s="1" t="n">
-        <f aca="false">MAX(I25,J25)</f>
-        <v>1000</v>
+        <v>7000</v>
       </c>
       <c r="D25" s="1" t="n">
-        <f aca="false">MAX(I25,K25)</f>
-        <v>1000</v>
+        <v>7000</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I25" s="1" t="n">
         <v>1000</v>
       </c>
       <c r="J25" s="0"/>
       <c r="K25" s="0"/>
+      <c r="L25" s="3" t="n">
+        <f aca="false">C25=D25</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C26" s="1" t="n">
         <f aca="false">MAX(I26,J26)</f>
@@ -1316,31 +1405,33 @@
         <v>0.2</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I26" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="J26" s="0"/>
       <c r="K26" s="0"/>
+      <c r="L26" s="3" t="n">
+        <f aca="false">C26=D26</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C27" s="1" t="n">
-        <f aca="false">MAX(I27,J27)</f>
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="D27" s="1" t="n">
-        <f aca="false">MAX(I27,K27)</f>
         <v>1</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I27" s="1" t="n">
         <v>0.8</v>
@@ -1351,37 +1442,43 @@
       <c r="K27" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="L27" s="3" t="n">
+        <f aca="false">C27=D27</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="s">
-        <v>78</v>
+      <c r="A28" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C28" s="1" t="n">
-        <f aca="false">MAX(I28,J28)</f>
-        <v>100000</v>
+        <v>1000</v>
       </c>
       <c r="D28" s="1" t="n">
-        <f aca="false">MAX(I28,K28)</f>
-        <v>100000</v>
+        <v>1000</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I28" s="1" t="n">
         <v>100000</v>
       </c>
       <c r="J28" s="0"/>
       <c r="K28" s="0"/>
+      <c r="L28" s="3" t="n">
+        <f aca="false">C28=D28</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C29" s="1" t="n">
         <v>0.3</v>
@@ -1390,24 +1487,28 @@
         <v>0.7</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I29" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="I29" s="5" t="n">
         <v>0.5</v>
       </c>
-      <c r="J29" s="4" t="n">
+      <c r="J29" s="5" t="n">
         <v>0.6</v>
       </c>
-      <c r="K29" s="4" t="n">
-        <v>1</v>
+      <c r="K29" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="L29" s="3" t="n">
+        <f aca="false">C29=D29</f>
+        <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C30" s="1" t="n">
         <f aca="false">MAX(I30,J30)</f>
@@ -1422,13 +1523,17 @@
       </c>
       <c r="J30" s="0"/>
       <c r="K30" s="0"/>
+      <c r="L30" s="3" t="n">
+        <f aca="false">C30=D30</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C31" s="1" t="n">
         <f aca="false">MAX(I31,J31)</f>
@@ -1444,13 +1549,17 @@
       </c>
       <c r="J31" s="0"/>
       <c r="K31" s="0"/>
+      <c r="L31" s="3" t="n">
+        <f aca="false">C31=D31</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C32" s="1" t="n">
         <f aca="false">MAX(I32,J32)</f>
@@ -1461,20 +1570,24 @@
         <v>0.25</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I32" s="1" t="n">
         <v>0.25</v>
       </c>
       <c r="J32" s="0"/>
       <c r="K32" s="0"/>
+      <c r="L32" s="3" t="n">
+        <f aca="false">C32=D32</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C33" s="1" t="n">
         <f aca="false">MAX(I33,J33)</f>
@@ -1485,31 +1598,33 @@
         <v>0.25</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I33" s="1" t="n">
         <v>0.25</v>
       </c>
       <c r="J33" s="0"/>
       <c r="K33" s="0"/>
+      <c r="L33" s="3" t="n">
+        <f aca="false">C33=D33</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C34" s="1" t="n">
-        <f aca="false">MAX(I34,J34)</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D34" s="1" t="n">
-        <f aca="false">MAX(I34,K34)</f>
         <v>1</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I34" s="1" t="n">
         <v>1</v>
@@ -1520,24 +1635,27 @@
       <c r="K34" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="L34" s="3" t="n">
+        <f aca="false">C34=D34</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C35" s="1" t="n">
-        <f aca="false">MAX(I35,J35)</f>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="D35" s="1" t="n">
         <f aca="false">MAX(I35,K35)</f>
         <v>0.25</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I35" s="1" t="n">
         <v>0.25</v>
@@ -1548,24 +1666,26 @@
       <c r="K35" s="1" t="n">
         <v>0.25</v>
       </c>
+      <c r="L35" s="3" t="n">
+        <f aca="false">C35=D35</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C36" s="1" t="n">
-        <f aca="false">MAX(I36,J36)</f>
-        <v>-0.1</v>
+        <v>-0.5</v>
       </c>
       <c r="D36" s="1" t="n">
-        <f aca="false">MAX(I36,K36)</f>
         <v>0</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I36" s="1" t="n">
         <v>-0.1</v>
@@ -1576,13 +1696,17 @@
       <c r="K36" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="L36" s="3" t="n">
+        <f aca="false">C36=D36</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C37" s="1" t="n">
         <f aca="false">MAX(I37,J37)</f>
@@ -1595,7 +1719,12 @@
       <c r="I37" s="1" t="n">
         <v>0</v>
       </c>
-    </row>
+      <c r="L37" s="3" t="n">
+        <f aca="false">C37=D37</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1612,33 +1741,33 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.59183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="7.69387755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1663,14 +1792,14 @@
       </c>
       <c r="B3" s="1" t="str">
         <f aca="false">"C."&amp;C3&amp;"-."&amp;D3</f>
-        <v>C.1-.0,4</v>
+        <v>C.1-.0,5</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="n">
-        <f aca="false">D2+0.1</f>
-        <v>0.4</v>
+        <f aca="false">D2+0.2</f>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1680,14 +1809,14 @@
       </c>
       <c r="B4" s="1" t="str">
         <f aca="false">"C."&amp;C4&amp;"-."&amp;D4</f>
-        <v>C.1-.0,5</v>
+        <v>C.1-.0,7</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D4" s="1" t="n">
-        <f aca="false">D3+0.1</f>
-        <v>0.5</v>
+        <f aca="false">D3+0.2</f>
+        <v>0.7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1697,14 +1826,14 @@
       </c>
       <c r="B5" s="1" t="str">
         <f aca="false">"C."&amp;C5&amp;"-."&amp;D5</f>
-        <v>C.1-.0,6</v>
+        <v>C.2-.0,3</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" s="1" t="n">
-        <f aca="false">D4+0.1</f>
-        <v>0.6</v>
+        <f aca="false">D2</f>
+        <v>0.3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1714,14 +1843,14 @@
       </c>
       <c r="B6" s="1" t="str">
         <f aca="false">"C."&amp;C6&amp;"-."&amp;D6</f>
-        <v>C.1-.0,7</v>
+        <v>C.2-.0,5</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" s="1" t="n">
-        <f aca="false">D5+0.1</f>
-        <v>0.7</v>
+        <f aca="false">D3</f>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1731,83 +1860,20 @@
       </c>
       <c r="B7" s="1" t="str">
         <f aca="false">"C."&amp;C7&amp;"-."&amp;D7</f>
-        <v>C.2-.0,3</v>
+        <v>C.2-.0,7</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D7" s="1" t="n">
-        <f aca="false">D2</f>
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
-        <f aca="false">A7+1</f>
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="str">
-        <f aca="false">"C."&amp;C8&amp;"-."&amp;D8</f>
-        <v>C.2-.0,4</v>
-      </c>
-      <c r="C8" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D8" s="1" t="n">
-        <f aca="false">D3</f>
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
-        <f aca="false">A8+1</f>
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="str">
-        <f aca="false">"C."&amp;C9&amp;"-."&amp;D9</f>
-        <v>C.2-.0,5</v>
-      </c>
-      <c r="C9" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D9" s="1" t="n">
         <f aca="false">D4</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
-        <f aca="false">A9+1</f>
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="str">
-        <f aca="false">"C."&amp;C10&amp;"-."&amp;D10</f>
-        <v>C.2-.0,6</v>
-      </c>
-      <c r="C10" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D10" s="1" t="n">
-        <f aca="false">D5</f>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="str">
-        <f aca="false">"C."&amp;C11&amp;"-."&amp;D11</f>
-        <v>C.2-.0,7</v>
-      </c>
-      <c r="C11" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D11" s="1" t="n">
-        <f aca="false">D6</f>
         <v>0.7</v>
       </c>
     </row>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1826,24 +1892,24 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
-        <v>102</v>
+      <c r="A1" s="6" t="s">
+        <v>103</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1875,155 +1941,155 @@
   </sheetPr>
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.484693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adicionando patentes ao modelo do R, lineralizando a relação entre patentes e performance
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/params.xlsx
+++ b/models/dissertation-model/modelo-R/params.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="151">
   <si>
     <t>Variavel</t>
   </si>
@@ -426,6 +426,60 @@
   </si>
   <si>
     <t>Replicação</t>
+  </si>
+  <si>
+    <t>aPeDLigado</t>
+  </si>
+  <si>
+    <t>Configuração: PeD Ligado</t>
+  </si>
+  <si>
+    <t>aOrcamentoPeD</t>
+  </si>
+  <si>
+    <t>aTempoMedioRealizacaoPeD</t>
+  </si>
+  <si>
+    <t>aCustoMedioPatente</t>
+  </si>
+  <si>
+    <t>aTempoMedioAvaliacao</t>
+  </si>
+  <si>
+    <t>aTaxaRejeicao</t>
+  </si>
+  <si>
+    <t>aTempoVencimentoPatentes</t>
+  </si>
+  <si>
+    <t>aTempodeInutilizacaoPatente</t>
+  </si>
+  <si>
+    <t>Percentual de Orçamento Direcionado a PeD</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>$ / patente</t>
+  </si>
+  <si>
+    <t>Tempo Médio para um investimento em PeD gerar uma patente.</t>
+  </si>
+  <si>
+    <t>Custo médio de obtenção de uma patente.</t>
+  </si>
+  <si>
+    <t>Tempo Médio para a rejeição ou concessão de uma patente.</t>
+  </si>
+  <si>
+    <t>Percentual de patentes solicitadas que são rejeitadas.</t>
+  </si>
+  <si>
+    <t>Tempo de Expiração de uma patente.</t>
+  </si>
+  <si>
+    <t>Tempo de Inutilização (após a expiração de uma patente).</t>
   </si>
 </sst>
 </file>
@@ -807,18 +861,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMK37"/>
+  <dimension ref="A1:AMK45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.42578125" style="1"/>
-    <col min="2" max="2" width="47" style="1"/>
-    <col min="3" max="3" width="9.85546875" style="1"/>
-    <col min="4" max="4" width="7.7109375" style="1"/>
+    <col min="2" max="2" width="56.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" style="1"/>
     <col min="6" max="7" width="7.7109375" style="1"/>
     <col min="8" max="8" width="11.5703125" style="1"/>
@@ -1958,12 +2012,153 @@
         <f>MAX(I37,K37)</f>
         <v>0</v>
       </c>
+      <c r="E37" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="I37" s="1">
         <v>0</v>
       </c>
       <c r="L37" s="3" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C38" s="3">
+        <v>1</v>
+      </c>
+      <c r="D38" s="1">
+        <v>1</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C39" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="D39" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C40" s="3">
+        <v>4</v>
+      </c>
+      <c r="D40" s="3">
+        <v>4</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C41" s="3">
+        <v>100000</v>
+      </c>
+      <c r="D41" s="3">
+        <v>100000</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C42" s="3">
+        <v>2</v>
+      </c>
+      <c r="D42" s="3">
+        <v>2</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C43" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="D43" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C44" s="1">
+        <f>20-2</f>
+        <v>18</v>
+      </c>
+      <c r="D44" s="3">
+        <f>20-2</f>
+        <v>18</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C45" s="3">
+        <v>10</v>
+      </c>
+      <c r="D45" s="3">
+        <v>10</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
patentes inseridas no modelo no R
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/params.xlsx
+++ b/models/dissertation-model/modelo-R/params.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="167">
   <si>
     <t>Variavel</t>
   </si>
@@ -480,6 +480,54 @@
   </si>
   <si>
     <t>Tempo de Inutilização (após a expiração de uma patente).</t>
+  </si>
+  <si>
+    <t>aPerfSlope</t>
+  </si>
+  <si>
+    <t>Melhoria em performance por patente que a empresa tem acesso.</t>
+  </si>
+  <si>
+    <t>Unidades de Performance / Patentes</t>
+  </si>
+  <si>
+    <t>aPerfMin</t>
+  </si>
+  <si>
+    <t>aPerfMax</t>
+  </si>
+  <si>
+    <t>aSensOfAttractToPerformance</t>
+  </si>
+  <si>
+    <t>aReferencePerformance</t>
+  </si>
+  <si>
+    <t>Índice de Performance Mínimo</t>
+  </si>
+  <si>
+    <t>Índice de Performance Máximo</t>
+  </si>
+  <si>
+    <t>aInitialInvestimentoNaoRealizadoPeD</t>
+  </si>
+  <si>
+    <t>aInitialPatentesRequisitadas</t>
+  </si>
+  <si>
+    <t>aInitialPatentesEmpresa</t>
+  </si>
+  <si>
+    <t>aInitialsPatentesEmDominioPublicoUteis</t>
+  </si>
+  <si>
+    <t>aInitialsInvestimentoPeDDepreciar</t>
+  </si>
+  <si>
+    <t>aPatentShare</t>
+  </si>
+  <si>
+    <t>Share de Patentes</t>
   </si>
 </sst>
 </file>
@@ -861,22 +909,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMK45"/>
+  <dimension ref="A1:AMK56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" style="1"/>
+    <col min="1" max="1" width="38.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="56.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" style="1"/>
     <col min="6" max="7" width="7.7109375" style="1"/>
     <col min="8" max="8" width="11.5703125" style="1"/>
-    <col min="9" max="9" width="7.28515625" style="1"/>
+    <col min="9" max="9" width="8.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="10.85546875" style="1"/>
     <col min="11" max="11" width="10.42578125" style="1"/>
     <col min="12" max="1025" width="7.7109375" style="1"/>
@@ -2039,6 +2087,9 @@
       <c r="E38" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="I38" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
@@ -2056,6 +2107,9 @@
       <c r="E39" s="3" t="s">
         <v>143</v>
       </c>
+      <c r="I39" s="3">
+        <v>1E-3</v>
+      </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
@@ -2073,6 +2127,9 @@
       <c r="E40" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="I40" s="3">
+        <v>4</v>
+      </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
@@ -2090,6 +2147,9 @@
       <c r="E41" s="3" t="s">
         <v>144</v>
       </c>
+      <c r="I41" s="3">
+        <v>100000</v>
+      </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
@@ -2107,6 +2167,9 @@
       <c r="E42" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="I42" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
@@ -2124,6 +2187,9 @@
       <c r="E43" s="3" t="s">
         <v>143</v>
       </c>
+      <c r="I43" s="3">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
@@ -2143,6 +2209,9 @@
       <c r="E44" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="I44" s="3">
+        <v>18</v>
+      </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
@@ -2159,6 +2228,181 @@
       </c>
       <c r="E45" s="3" t="s">
         <v>24</v>
+      </c>
+      <c r="I45" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C46" s="1">
+        <f>1/30</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="D46" s="1">
+        <f>1/30</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="I46" s="1">
+        <f>1/30</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C47" s="3">
+        <v>0</v>
+      </c>
+      <c r="D47" s="3">
+        <v>0</v>
+      </c>
+      <c r="I47" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C48" s="3">
+        <v>10</v>
+      </c>
+      <c r="D48" s="3">
+        <v>10</v>
+      </c>
+      <c r="I48" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C49" s="3">
+        <v>-4</v>
+      </c>
+      <c r="D49" s="3">
+        <v>-4</v>
+      </c>
+      <c r="I49" s="3">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C50" s="3">
+        <v>10</v>
+      </c>
+      <c r="D50" s="3">
+        <v>10</v>
+      </c>
+      <c r="I50" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C51" s="3">
+        <v>1000</v>
+      </c>
+      <c r="D51" s="3">
+        <v>1000</v>
+      </c>
+      <c r="I51" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C52" s="3">
+        <v>100</v>
+      </c>
+      <c r="D52" s="3">
+        <v>100</v>
+      </c>
+      <c r="I52" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C53" s="3">
+        <v>100</v>
+      </c>
+      <c r="D53" s="3">
+        <v>100</v>
+      </c>
+      <c r="I53" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C54" s="3">
+        <v>20</v>
+      </c>
+      <c r="D54" s="3">
+        <v>20</v>
+      </c>
+      <c r="I54" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C55" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="D55" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="I55" s="3">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C56" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D56" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="I56" s="3">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tentando realizar calibração- os resultados do R não fecham com o iThink. Verificar a origem das inconsistências antes de calibrar
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/params.xlsx
+++ b/models/dissertation-model/modelo-R/params.xlsx
@@ -17,7 +17,7 @@
     <sheet name="configs" sheetId="3" r:id="rId3"/>
     <sheet name="VariableNames" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="171">
   <si>
     <t>Variavel</t>
   </si>
@@ -528,6 +528,18 @@
   </si>
   <si>
     <t>Share de Patentes</t>
+  </si>
+  <si>
+    <t>aInitialSharePlayers</t>
+  </si>
+  <si>
+    <t>aInitialReorderShare</t>
+  </si>
+  <si>
+    <t>aTotalInitialInstalledBase</t>
+  </si>
+  <si>
+    <t>aInitialIndustryShipments</t>
   </si>
 </sst>
 </file>
@@ -909,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMK56"/>
+  <dimension ref="A1:AMK60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,7 +992,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>14</v>
@@ -999,7 +1011,7 @@
       <c r="K2"/>
       <c r="L2" s="3" t="b">
         <f t="shared" ref="L2:L37" si="1">C2=D2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2403,6 +2415,50 @@
       </c>
       <c r="I56" s="3">
         <v>0.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C57" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D57" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C58" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="D58" s="3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C59" s="3">
+        <v>2500</v>
+      </c>
+      <c r="D59" s="3">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C60" s="3">
+        <v>1831</v>
+      </c>
+      <c r="D60" s="3">
+        <v>1831</v>
       </c>
     </row>
   </sheetData>
@@ -2413,10 +2469,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMK7"/>
+  <dimension ref="A1:AMK2"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2424,7 +2480,7 @@
     <col min="1" max="1" width="4.5703125" style="1"/>
     <col min="2" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="24.28515625" style="1"/>
-    <col min="4" max="4" width="17.85546875" style="1"/>
+    <col min="4" max="4" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="1025" width="7.7109375" style="1"/>
   </cols>
   <sheetData>
@@ -2447,99 +2503,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="str">
-        <f t="shared" ref="B2:B7" si="0">"C."&amp;C2&amp;"-."&amp;D2</f>
-        <v>C.1-.0,3</v>
+        <f t="shared" ref="B2" si="0">"C."&amp;C2&amp;"-."&amp;D2</f>
+        <v>C.1-.0,5</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
       </c>
       <c r="D2" s="1">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <f>A2+1</f>
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>C.1-.0,5</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
-        <f>D2+0.2</f>
         <v>0.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <f>A3+1</f>
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>C.1-.0,7</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1">
-        <f>D3+0.2</f>
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <f>A4+1</f>
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>C.2-.0,3</v>
-      </c>
-      <c r="C5" s="1">
-        <v>2</v>
-      </c>
-      <c r="D5" s="1">
-        <f>D2</f>
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <f>A5+1</f>
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>C.2-.0,5</v>
-      </c>
-      <c r="C6" s="1">
-        <v>2</v>
-      </c>
-      <c r="D6" s="1">
-        <f>D3</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <f>A6+1</f>
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>C.2-.0,7</v>
-      </c>
-      <c r="C7" s="1">
-        <v>2</v>
-      </c>
-      <c r="D7" s="1">
-        <f>D4</f>
-        <v>0.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>